<commit_message>
Visual for state change, start county
</commit_message>
<xml_diff>
--- a/tabulated_forest.xlsx
+++ b/tabulated_forest.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbouf\Documents\UVM\Maryland_Technical_Forest\MD_Forest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C91C11E-2450-4FAD-86CE-785216D84D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4DDFC3-CCF6-4711-957B-C891FDD309D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D00C5090-3B11-4247-BA8E-6E7E97698597}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{D00C5090-3B11-4247-BA8E-6E7E97698597}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
   <si>
     <t>Year</t>
   </si>
@@ -49,6 +50,81 @@
   </si>
   <si>
     <t>Geography</t>
+  </si>
+  <si>
+    <t>COUNTY</t>
+  </si>
+  <si>
+    <t>Allegany</t>
+  </si>
+  <si>
+    <t>Anne Arundel</t>
+  </si>
+  <si>
+    <t>Baltimore</t>
+  </si>
+  <si>
+    <t>Baltimore City</t>
+  </si>
+  <si>
+    <t>Calvert</t>
+  </si>
+  <si>
+    <t>Caroline</t>
+  </si>
+  <si>
+    <t>Carroll</t>
+  </si>
+  <si>
+    <t>Cecil</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Dorchester</t>
+  </si>
+  <si>
+    <t>Frederick</t>
+  </si>
+  <si>
+    <t>Garrett</t>
+  </si>
+  <si>
+    <t>Harford</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>Kent</t>
+  </si>
+  <si>
+    <t>Montgomery</t>
+  </si>
+  <si>
+    <t>Prince George's</t>
+  </si>
+  <si>
+    <t>Queen Anne's</t>
+  </si>
+  <si>
+    <t>Somerset</t>
+  </si>
+  <si>
+    <t>St. Mary's</t>
+  </si>
+  <si>
+    <t>Talbot</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Wicomico</t>
+  </si>
+  <si>
+    <t>Worcester</t>
   </si>
 </sst>
 </file>
@@ -90,10 +166,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,7 +491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB07B336-991B-4A9E-A2FC-315364CBDDEA}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -576,4 +657,1000 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C3ABAE-2C2E-4C52-BD28-A2FB9EC08C44}">
+  <dimension ref="A1:F49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4">
+        <v>2000</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2005</v>
+      </c>
+      <c r="D1" s="4">
+        <v>2010</v>
+      </c>
+      <c r="E1" s="4">
+        <v>2015</v>
+      </c>
+      <c r="F1" s="4">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4">
+        <v>203053241.44941899</v>
+      </c>
+      <c r="C2" s="4">
+        <v>198458222.09999999</v>
+      </c>
+      <c r="D2" s="4">
+        <v>202549938.59999999</v>
+      </c>
+      <c r="E2" s="4">
+        <v>203107652.59999999</v>
+      </c>
+      <c r="F2" s="4">
+        <v>202197173.09999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4">
+        <v>362034380.35227799</v>
+      </c>
+      <c r="C3" s="4">
+        <v>359762716</v>
+      </c>
+      <c r="D3" s="4">
+        <v>354884758.80000001</v>
+      </c>
+      <c r="E3" s="4">
+        <v>359295687.19999999</v>
+      </c>
+      <c r="F3" s="4">
+        <v>358471358.69999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4">
+        <v>713454964.367082</v>
+      </c>
+      <c r="C4" s="4">
+        <v>704971363.5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>700300168.60000002</v>
+      </c>
+      <c r="E4" s="4">
+        <v>697048197.20000005</v>
+      </c>
+      <c r="F4" s="4">
+        <v>691508238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4">
+        <v>144453369.13813299</v>
+      </c>
+      <c r="C5" s="4">
+        <v>144467878.80000001</v>
+      </c>
+      <c r="D5" s="4">
+        <v>145165248</v>
+      </c>
+      <c r="E5" s="4">
+        <v>145302182.69999999</v>
+      </c>
+      <c r="F5" s="4">
+        <v>145572424.59999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4">
+        <v>155365519.79849201</v>
+      </c>
+      <c r="C6" s="4">
+        <v>154579279.09999999</v>
+      </c>
+      <c r="D6" s="4">
+        <v>152907950.80000001</v>
+      </c>
+      <c r="E6" s="4">
+        <v>152633174.59999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>151465149.19999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4">
+        <v>539858997.90315402</v>
+      </c>
+      <c r="C7" s="4">
+        <v>540704184</v>
+      </c>
+      <c r="D7" s="4">
+        <v>536876361.5</v>
+      </c>
+      <c r="E7" s="4">
+        <v>534507664</v>
+      </c>
+      <c r="F7" s="4">
+        <v>533155547.60000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4">
+        <v>761974269.34349406</v>
+      </c>
+      <c r="C8" s="4">
+        <v>748521119.29999995</v>
+      </c>
+      <c r="D8" s="4">
+        <v>740728539.60000002</v>
+      </c>
+      <c r="E8" s="4">
+        <v>734316188.79999995</v>
+      </c>
+      <c r="F8" s="4">
+        <v>718579585.29999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
+        <v>495948315.02064699</v>
+      </c>
+      <c r="C9" s="4">
+        <v>494001303.69999999</v>
+      </c>
+      <c r="D9" s="4">
+        <v>494589850.69999999</v>
+      </c>
+      <c r="E9" s="4">
+        <v>493056363.80000001</v>
+      </c>
+      <c r="F9" s="4">
+        <v>490565241.30000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4">
+        <v>325582555.54185897</v>
+      </c>
+      <c r="C10" s="4">
+        <v>328737493.80000001</v>
+      </c>
+      <c r="D10" s="4">
+        <v>327577630</v>
+      </c>
+      <c r="E10" s="4">
+        <v>329265281.69999999</v>
+      </c>
+      <c r="F10" s="4">
+        <v>325569859.60000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4">
+        <v>950659346.98815</v>
+      </c>
+      <c r="C11" s="4">
+        <v>942854978.29999995</v>
+      </c>
+      <c r="D11" s="4">
+        <v>936380961.5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>931922876.89999998</v>
+      </c>
+      <c r="F11" s="4">
+        <v>930436546.39999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1051578376.84255</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1040132090</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1035927924</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1028560658</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1017315693</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4">
+        <v>435173811.50487798</v>
+      </c>
+      <c r="C13" s="4">
+        <v>436482399</v>
+      </c>
+      <c r="D13" s="4">
+        <v>440677496.60000002</v>
+      </c>
+      <c r="E13" s="4">
+        <v>441154500.69999999</v>
+      </c>
+      <c r="F13" s="4">
+        <v>437243247.89999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4">
+        <v>583975536.19993198</v>
+      </c>
+      <c r="C14" s="4">
+        <v>576409669.60000002</v>
+      </c>
+      <c r="D14" s="4">
+        <v>575667864.60000002</v>
+      </c>
+      <c r="E14" s="4">
+        <v>572981768.89999998</v>
+      </c>
+      <c r="F14" s="4">
+        <v>566930345.20000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4">
+        <v>296202362.98021299</v>
+      </c>
+      <c r="C15" s="4">
+        <v>288904017.69999999</v>
+      </c>
+      <c r="D15" s="4">
+        <v>283468346.60000002</v>
+      </c>
+      <c r="E15" s="4">
+        <v>280015960.80000001</v>
+      </c>
+      <c r="F15" s="4">
+        <v>273612678.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4">
+        <v>529768455.19578201</v>
+      </c>
+      <c r="C16" s="4">
+        <v>528611312</v>
+      </c>
+      <c r="D16" s="4">
+        <v>526122910</v>
+      </c>
+      <c r="E16" s="4">
+        <v>524838807.5</v>
+      </c>
+      <c r="F16" s="4">
+        <v>522956182.60000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4">
+        <v>531387186.09653401</v>
+      </c>
+      <c r="C17" s="4">
+        <v>518433711.5</v>
+      </c>
+      <c r="D17" s="4">
+        <v>511484504.30000001</v>
+      </c>
+      <c r="E17" s="4">
+        <v>510851521.5</v>
+      </c>
+      <c r="F17" s="4">
+        <v>496372721.80000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="4">
+        <v>450569438.67689699</v>
+      </c>
+      <c r="C18" s="4">
+        <v>456356968.39999998</v>
+      </c>
+      <c r="D18" s="4">
+        <v>448962496.89999998</v>
+      </c>
+      <c r="E18" s="4">
+        <v>454159665.89999998</v>
+      </c>
+      <c r="F18" s="4">
+        <v>442427721</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="4">
+        <v>666806495.15999806</v>
+      </c>
+      <c r="C19" s="4">
+        <v>664985536.29999995</v>
+      </c>
+      <c r="D19" s="4">
+        <v>660954578.89999998</v>
+      </c>
+      <c r="E19" s="4">
+        <v>657662706</v>
+      </c>
+      <c r="F19" s="4">
+        <v>654018974.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="4">
+        <v>474762437.53977799</v>
+      </c>
+      <c r="C20" s="4">
+        <v>460802357.19999999</v>
+      </c>
+      <c r="D20" s="4">
+        <v>450898626</v>
+      </c>
+      <c r="E20" s="4">
+        <v>442999944.69999999</v>
+      </c>
+      <c r="F20" s="4">
+        <v>442014196.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="4">
+        <v>343951750.57021701</v>
+      </c>
+      <c r="C21" s="4">
+        <v>343829325.5</v>
+      </c>
+      <c r="D21" s="4">
+        <v>341441584.10000002</v>
+      </c>
+      <c r="E21" s="4">
+        <v>339942557.69999999</v>
+      </c>
+      <c r="F21" s="4">
+        <v>338755488.39999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="4">
+        <v>475108855.02105898</v>
+      </c>
+      <c r="C22" s="4">
+        <v>473737694.69999999</v>
+      </c>
+      <c r="D22" s="4">
+        <v>467433259.30000001</v>
+      </c>
+      <c r="E22" s="4">
+        <v>463164706.69999999</v>
+      </c>
+      <c r="F22" s="4">
+        <v>461173259.60000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="4">
+        <v>651995787.55715799</v>
+      </c>
+      <c r="C23" s="4">
+        <v>646871166.60000002</v>
+      </c>
+      <c r="D23" s="4">
+        <v>646390535.10000002</v>
+      </c>
+      <c r="E23" s="4">
+        <v>637177825.10000002</v>
+      </c>
+      <c r="F23" s="4">
+        <v>632285358.39999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="4">
+        <v>488397864.89198798</v>
+      </c>
+      <c r="C24" s="4">
+        <v>478848712.89999998</v>
+      </c>
+      <c r="D24" s="4">
+        <v>463136594.30000001</v>
+      </c>
+      <c r="E24" s="4">
+        <v>453286367.39999998</v>
+      </c>
+      <c r="F24" s="4">
+        <v>451897070.10000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="4">
+        <v>567624086.97223103</v>
+      </c>
+      <c r="C25" s="4">
+        <v>557436511.10000002</v>
+      </c>
+      <c r="D25" s="4">
+        <v>539580594.29999995</v>
+      </c>
+      <c r="E25" s="4">
+        <v>528716506.80000001</v>
+      </c>
+      <c r="F25" s="4">
+        <v>528651213.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="4">
+        <v>893783400.41486299</v>
+      </c>
+      <c r="C26" s="4">
+        <v>898378419.70000005</v>
+      </c>
+      <c r="D26" s="4">
+        <v>894286703.29999995</v>
+      </c>
+      <c r="E26" s="4">
+        <v>893728989.29999995</v>
+      </c>
+      <c r="F26" s="4">
+        <v>894639468.70000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="4">
+        <v>710103239.20788002</v>
+      </c>
+      <c r="C27" s="4">
+        <v>712374903.60000002</v>
+      </c>
+      <c r="D27" s="4">
+        <v>717252860.70000005</v>
+      </c>
+      <c r="E27" s="4">
+        <v>712841932.39999998</v>
+      </c>
+      <c r="F27" s="4">
+        <v>713666260.89999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="4">
+        <v>839203603.22011995</v>
+      </c>
+      <c r="C28" s="4">
+        <v>847687204.10000002</v>
+      </c>
+      <c r="D28" s="4">
+        <v>852358399</v>
+      </c>
+      <c r="E28" s="4">
+        <v>855610370.39999998</v>
+      </c>
+      <c r="F28" s="4">
+        <v>861150329.60000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="4">
+        <v>66125837.434722699</v>
+      </c>
+      <c r="C29" s="4">
+        <v>66111327.799999997</v>
+      </c>
+      <c r="D29" s="4">
+        <v>65413958.579999998</v>
+      </c>
+      <c r="E29" s="4">
+        <v>65277023.920000002</v>
+      </c>
+      <c r="F29" s="4">
+        <v>65006782.009999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="4">
+        <v>399514575.381998</v>
+      </c>
+      <c r="C30" s="4">
+        <v>400300816.10000002</v>
+      </c>
+      <c r="D30" s="4">
+        <v>401972144.39999998</v>
+      </c>
+      <c r="E30" s="4">
+        <v>402246920.60000002</v>
+      </c>
+      <c r="F30" s="4">
+        <v>403414946</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="4">
+        <v>289386463.00819802</v>
+      </c>
+      <c r="C31" s="4">
+        <v>288541276.89999998</v>
+      </c>
+      <c r="D31" s="4">
+        <v>292369099.39999998</v>
+      </c>
+      <c r="E31" s="4">
+        <v>294737796.89999998</v>
+      </c>
+      <c r="F31" s="4">
+        <v>296089913.30000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="4">
+        <v>402423756.74312401</v>
+      </c>
+      <c r="C32" s="4">
+        <v>415876906.80000001</v>
+      </c>
+      <c r="D32" s="4">
+        <v>423669486.5</v>
+      </c>
+      <c r="E32" s="4">
+        <v>430081837.30000001</v>
+      </c>
+      <c r="F32" s="4">
+        <v>445818440.80000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="4">
+        <v>407273601.48106098</v>
+      </c>
+      <c r="C33" s="4">
+        <v>409220612.80000001</v>
+      </c>
+      <c r="D33" s="4">
+        <v>408632065.80000001</v>
+      </c>
+      <c r="E33" s="4">
+        <v>410165552.69999999</v>
+      </c>
+      <c r="F33" s="4">
+        <v>412656675.19999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="4">
+        <v>866575118.50156295</v>
+      </c>
+      <c r="C34" s="4">
+        <v>863420180.20000005</v>
+      </c>
+      <c r="D34" s="4">
+        <v>864580044</v>
+      </c>
+      <c r="E34" s="4">
+        <v>862892392.29999995</v>
+      </c>
+      <c r="F34" s="4">
+        <v>866587814.39999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="4">
+        <v>454136994.62286597</v>
+      </c>
+      <c r="C35" s="4">
+        <v>461941363.30000001</v>
+      </c>
+      <c r="D35" s="4">
+        <v>468415380.10000002</v>
+      </c>
+      <c r="E35" s="4">
+        <v>472873464.69999999</v>
+      </c>
+      <c r="F35" s="4">
+        <v>474359795.19999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="4">
+        <v>664484953.92418694</v>
+      </c>
+      <c r="C36" s="4">
+        <v>675931240.39999998</v>
+      </c>
+      <c r="D36" s="4">
+        <v>680135406.5</v>
+      </c>
+      <c r="E36" s="4">
+        <v>687502672.5</v>
+      </c>
+      <c r="F36" s="4">
+        <v>698747637.89999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1264713999.33093</v>
+      </c>
+      <c r="C37" s="4">
+        <v>1263405412</v>
+      </c>
+      <c r="D37" s="4">
+        <v>1259210314</v>
+      </c>
+      <c r="E37" s="4">
+        <v>1258733310</v>
+      </c>
+      <c r="F37" s="4">
+        <v>1262644563</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="4">
+        <v>550981538.23800802</v>
+      </c>
+      <c r="C38" s="4">
+        <v>558547404.89999998</v>
+      </c>
+      <c r="D38" s="4">
+        <v>559289209.79999995</v>
+      </c>
+      <c r="E38" s="4">
+        <v>561975305.60000002</v>
+      </c>
+      <c r="F38" s="4">
+        <v>568026729.29999995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="4">
+        <v>356018323.88416398</v>
+      </c>
+      <c r="C39" s="4">
+        <v>363316669.10000002</v>
+      </c>
+      <c r="D39" s="4">
+        <v>368752340.30000001</v>
+      </c>
+      <c r="E39" s="4">
+        <v>372204726</v>
+      </c>
+      <c r="F39" s="4">
+        <v>378608008.30000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="4">
+        <v>195826537.500911</v>
+      </c>
+      <c r="C40" s="4">
+        <v>196983680.69999999</v>
+      </c>
+      <c r="D40" s="4">
+        <v>199472082.69999999</v>
+      </c>
+      <c r="E40" s="4">
+        <v>200756185.19999999</v>
+      </c>
+      <c r="F40" s="4">
+        <v>202638810.09999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="4">
+        <v>755617236.50636995</v>
+      </c>
+      <c r="C41" s="4">
+        <v>768570711.10000002</v>
+      </c>
+      <c r="D41" s="4">
+        <v>775519918.29999995</v>
+      </c>
+      <c r="E41" s="4">
+        <v>776152901.10000002</v>
+      </c>
+      <c r="F41" s="4">
+        <v>790631700.79999995</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="4">
+        <v>805194837.81957495</v>
+      </c>
+      <c r="C42" s="4">
+        <v>799407308.10000002</v>
+      </c>
+      <c r="D42" s="4">
+        <v>806801779.60000002</v>
+      </c>
+      <c r="E42" s="4">
+        <v>801604610.60000002</v>
+      </c>
+      <c r="F42" s="4">
+        <v>813336555.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="4">
+        <v>296670298.63555598</v>
+      </c>
+      <c r="C43" s="4">
+        <v>298491257.5</v>
+      </c>
+      <c r="D43" s="4">
+        <v>302522214.89999998</v>
+      </c>
+      <c r="E43" s="4">
+        <v>305814087.80000001</v>
+      </c>
+      <c r="F43" s="4">
+        <v>309457819.30000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="4">
+        <v>352761818.18971199</v>
+      </c>
+      <c r="C44" s="4">
+        <v>366721898.60000002</v>
+      </c>
+      <c r="D44" s="4">
+        <v>376625629.80000001</v>
+      </c>
+      <c r="E44" s="4">
+        <v>384524311.10000002</v>
+      </c>
+      <c r="F44" s="4">
+        <v>385510059.19999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="4">
+        <v>587763457.19289398</v>
+      </c>
+      <c r="C45" s="4">
+        <v>587885882.20000005</v>
+      </c>
+      <c r="D45" s="4">
+        <v>590273623.70000005</v>
+      </c>
+      <c r="E45" s="4">
+        <v>591772650.10000002</v>
+      </c>
+      <c r="F45" s="4">
+        <v>592959719.39999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="4">
+        <v>222966805.510818</v>
+      </c>
+      <c r="C46" s="4">
+        <v>224337965.80000001</v>
+      </c>
+      <c r="D46" s="4">
+        <v>230642401.19999999</v>
+      </c>
+      <c r="E46" s="4">
+        <v>234910953.80000001</v>
+      </c>
+      <c r="F46" s="4">
+        <v>236902400.90000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="4">
+        <v>533745001.41415501</v>
+      </c>
+      <c r="C47" s="4">
+        <v>538869622.29999995</v>
+      </c>
+      <c r="D47" s="4">
+        <v>539350253.89999998</v>
+      </c>
+      <c r="E47" s="4">
+        <v>548562963.79999995</v>
+      </c>
+      <c r="F47" s="4">
+        <v>553455430.60000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="4">
+        <v>484858421.35942101</v>
+      </c>
+      <c r="C48" s="4">
+        <v>494407573.39999998</v>
+      </c>
+      <c r="D48" s="4">
+        <v>510119691.89999998</v>
+      </c>
+      <c r="E48" s="4">
+        <v>519969918.80000001</v>
+      </c>
+      <c r="F48" s="4">
+        <v>521359216.19999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="4">
+        <v>653657140.50403595</v>
+      </c>
+      <c r="C49" s="4">
+        <v>663844716.39999998</v>
+      </c>
+      <c r="D49" s="4">
+        <v>681700633.20000005</v>
+      </c>
+      <c r="E49" s="4">
+        <v>692564720.70000005</v>
+      </c>
+      <c r="F49" s="4">
+        <v>692630014</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Having issue reading in county data
</commit_message>
<xml_diff>
--- a/tabulated_forest.xlsx
+++ b/tabulated_forest.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbouf\Documents\UVM\Maryland_Technical_Forest\MD_Forest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4DDFC3-CCF6-4711-957B-C891FDD309D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B78409-F7A6-49C3-B81D-A69B40266DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{D00C5090-3B11-4247-BA8E-6E7E97698597}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D00C5090-3B11-4247-BA8E-6E7E97698597}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="state" sheetId="1" r:id="rId1"/>
+    <sheet name="county" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -664,7 +664,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>